<commit_message>
commit 21/3 1-edit mobile number 2-Resend Otp
</commit_message>
<xml_diff>
--- a/src/test/testdata/TestData.xlsx
+++ b/src/test/testdata/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>111633332215&amp;</t>
+  </si>
+  <si>
+    <t>Amira</t>
+  </si>
+  <si>
+    <t>1116332215&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03-edit Mobile Nuber while login </t>
   </si>
 </sst>
 </file>
@@ -117,11 +126,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,15 +415,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
   </cols>
@@ -447,6 +459,17 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit 27-3 add driver cycle with start joborder - pickup vehicle -completer jobOrderID
</commit_message>
<xml_diff>
--- a/src/test/testdata/TestData.xlsx
+++ b/src/test/testdata/TestData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="8616" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Locations" sheetId="2" r:id="rId2"/>
+    <sheet name="Request" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -417,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,4 +530,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>